<commit_message>
developing dataframes pertaining to positive yearly earnings
</commit_message>
<xml_diff>
--- a/msft_and_nflx_yearly_earnings_per_share_merge.xlsx
+++ b/msft_and_nflx_yearly_earnings_per_share_merge.xlsx
@@ -1,15 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27231"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/25ac2033dcfcea55/Desktop/ALIENWARE - 2023-04_24 - Onwards/Python/Stock Market Data/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="1" documentId="11_6B450C373308AA474A3C3467E833F2B47452296D" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{34179100-C950-40C8-9646-4C46C3225272}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="1950" yWindow="1950" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
@@ -82,8 +88,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -146,13 +152,21 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -190,7 +204,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -224,6 +238,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -258,9 +273,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -433,14 +449,31 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2:J4"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="22.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="26.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="5" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="20" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="22.7109375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="26.140625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:13">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -481,7 +514,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:13">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1107</v>
       </c>
@@ -495,7 +528,7 @@
         <v>2.61</v>
       </c>
       <c r="E2">
-        <v>8376628352.49</v>
+        <v>8376628352.4899998</v>
       </c>
       <c r="F2" t="s">
         <v>17</v>
@@ -513,7 +546,7 @@
         <v>1.93</v>
       </c>
       <c r="K2">
-        <v>58239896.3731</v>
+        <v>58239896.373099998</v>
       </c>
       <c r="L2" t="s">
         <v>17</v>
@@ -522,7 +555,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="3" spans="1:13">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1108</v>
       </c>
@@ -536,7 +569,7 @@
         <v>2.66</v>
       </c>
       <c r="E3">
-        <v>8298496240.6</v>
+        <v>8298496240.6000004</v>
       </c>
       <c r="F3" t="s">
         <v>17</v>
@@ -551,7 +584,7 @@
         <v>19</v>
       </c>
       <c r="J3">
-        <v>4.44</v>
+        <v>4.4400000000000004</v>
       </c>
       <c r="K3">
         <v>60089864.8649</v>
@@ -563,7 +596,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="4" spans="1:13">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>1109</v>
       </c>
@@ -577,7 +610,7 @@
         <v>1.49</v>
       </c>
       <c r="E4">
-        <v>8183221476.51</v>
+        <v>8183221476.5100002</v>
       </c>
       <c r="F4" t="s">
         <v>17</v>
@@ -592,7 +625,7 @@
         <v>19</v>
       </c>
       <c r="J4">
-        <v>0.29</v>
+        <v>0.28999999999999998</v>
       </c>
       <c r="K4">
         <v>422900000</v>

</xml_diff>